<commit_message>
Changes to be committed: 	modified:   src/infrastructure/services/nl_folha_gateway.py 	modified:   src/infrastructure/services/preenchimento_gateway.py 	modified:   tests/core/usecases/test_preenchimento_folha_usecase.py 	modified:   tests/fixtures/TEMPLATES/TEMPLATES_NL_FINANCEIRO.xlsx 	modified:   tests/mocks/siggo_service_mock.py
</commit_message>
<xml_diff>
--- a/tests/fixtures/TEMPLATES/TEMPLATES_NL_FINANCEIRO.xlsx
+++ b/tests/fixtures/TEMPLATES/TEMPLATES_NL_FINANCEIRO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tcdf.sharepoint.com/sites/SECON/Shared Documents/General/ANO_ATUAL/FOLHA_DE_PAGAMENTO_2025/TEMPLATES/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willyanmarques\Documents\Dev\preenchimento\tests\fixtures\TEMPLATES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="892" documentId="8_{25A6B9ED-1607-4154-B84C-B2B55EBDC884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E89D34C-07A6-45CA-9080-95312E80B25E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903D792A-FF2F-4DC1-9C03-1C74EC833F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="890" firstSheet="9" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="890" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PRINCIPAL" sheetId="3" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="140">
   <si>
     <t>31901101</t>
   </si>
@@ -467,6 +467,9 @@
   </si>
   <si>
     <t>tudo que for proventos de adiantamento de férias</t>
+  </si>
+  <si>
+    <t>33909300</t>
   </si>
 </sst>
 </file>
@@ -3050,7 +3053,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB61321-D9B8-4290-9E0D-73E516A2656E}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8:J10"/>
     </sheetView>
   </sheetViews>
@@ -3388,7 +3391,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3525,7 +3528,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3620,8 +3623,8 @@
       <c r="C8" s="2">
         <v>329110300</v>
       </c>
-      <c r="D8" s="2">
-        <v>33900805</v>
+      <c r="D8" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="E8" s="2">
         <v>100000000</v>
@@ -3725,8 +3728,8 @@
       <c r="C13" s="2">
         <v>211110101</v>
       </c>
-      <c r="D13" s="2">
-        <v>33900800</v>
+      <c r="D13" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="E13" s="2">
         <v>100000000</v>
@@ -4438,8 +4441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A17AD1A-D88B-4100-8FDE-E6ACE989C91F}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4595,8 +4598,8 @@
       <c r="C11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="2">
-        <v>33909300</v>
+      <c r="D11" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="E11" s="2">
         <v>100000000</v>
@@ -4619,8 +4622,8 @@
       <c r="C12" s="2">
         <v>211110101</v>
       </c>
-      <c r="D12" s="2">
-        <v>33909300</v>
+      <c r="D12" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="E12" s="2">
         <v>100000000</v>
@@ -4640,11 +4643,11 @@
       <c r="B13" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="2">
-        <v>211110101</v>
-      </c>
-      <c r="D13" s="2">
-        <v>33909300</v>
+      <c r="C13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="E13" s="2">
         <v>100000000</v>
@@ -4667,15 +4670,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="5f1ce42f-c57e-4699-9768-bf8c2a029303">
@@ -4685,6 +4679,15 @@
     <_Flow_SignoffStatus xmlns="5f1ce42f-c57e-4699-9768-bf8c2a029303" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4943,14 +4946,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{577AEBCC-ECF2-44EB-912A-AE3383D52A49}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3AE49084-5719-49CD-A008-AB879E7F1353}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4961,6 +4956,29 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{577AEBCC-ECF2-44EB-912A-AE3383D52A49}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE32D99A-2938-463B-82B7-51126764D078}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE32D99A-2938-463B-82B7-51126764D078}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="5f1ce42f-c57e-4699-9768-bf8c2a029303"/>
+    <ds:schemaRef ds:uri="a6d483d6-7cde-454f-9700-1dca77a67851"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>